<commit_message>
Fixed issue with giving description for education.
</commit_message>
<xml_diff>
--- a/Documentatie/CV_BurndownChart.xlsx
+++ b/Documentatie/CV_BurndownChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CVTemplater\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C7AFD4-DF90-4463-96EC-CF8E05B585A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9032DABD-4CE4-407B-9943-2126D3A9E7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E34AC782-7D53-43E9-8047-0B626BB00436}"/>
   </bookViews>
@@ -321,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,12 +349,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -468,9 +462,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2531,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B203C6C7-E02C-4509-B8EE-0C7EEB5D0B6F}">
   <dimension ref="B2:BK25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="BK16" sqref="BK16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2546,48 +2537,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:63" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2772,8 +2763,8 @@
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
@@ -3680,7 +3671,7 @@
       <c r="C15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>3</v>
       </c>
       <c r="E15" s="2"/>
@@ -4036,10 +4027,10 @@
       </c>
     </row>
     <row r="19" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="9">
         <v>1</v>
       </c>
@@ -4110,10 +4101,10 @@
       <c r="BK19" s="2"/>
     </row>
     <row r="20" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="9">
         <v>1</v>
       </c>
@@ -4184,10 +4175,10 @@
       <c r="BK20" s="2"/>
     </row>
     <row r="21" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="9">
         <v>2</v>
       </c>
@@ -4256,10 +4247,10 @@
       <c r="BK21" s="2"/>
     </row>
     <row r="22" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="9">
         <v>1</v>
       </c>
@@ -4330,10 +4321,10 @@
       </c>
     </row>
     <row r="23" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="9">
         <v>5</v>
       </c>
@@ -4408,10 +4399,10 @@
       <c r="BK23" s="2"/>
     </row>
     <row r="24" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="7">
         <f>D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18+D19+D20+D21+D22+D23</f>
         <v>60</v>
@@ -4654,10 +4645,10 @@
       </c>
     </row>
     <row r="25" spans="2:63" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="7">
         <f>D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18+D19+D20+D21+D22+D23</f>
         <v>60</v>

</xml_diff>